<commit_message>
Added more graphs from more experiments run, added several more batch files, and modified source .py scripts extensively to work with newly presented files as well as run the required experiments.
</commit_message>
<xml_diff>
--- a/project_files/documentation/RNN Results.xlsx
+++ b/project_files/documentation/RNN Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dheat\Dropbox\Imperial\Individual Project\indiv_proj\project_files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6290C72C-F411-434E-A33C-C924214FE101}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E39A13-1CFE-4536-9BE1-6AD7EE21191E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8778" xr2:uid="{F111C118-2C3B-40EB-A3AA-5A6786E31AB7}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="406">
   <si>
     <t>Notes</t>
   </si>
@@ -1062,6 +1062,192 @@
   </si>
   <si>
     <t>python ext_raw_measures.py allmatfiles all jointAngle</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA AD all overall --seq_len=7 --seq_overlap=0.857143</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA AD all overall --seq_len=3 --seq_overlap=0.67</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA AD all overall --seq_len=5 --seq_overlap=0.8</t>
+  </si>
+  <si>
+    <t>Stat values from NSAA\AD w/ seq_len=7 (w/ scaling seq_overlap) to perform overall NSAA score regression</t>
+  </si>
+  <si>
+    <t>Stat values from NSAA\AD w/ seq_len=5 (w/ scaling seq_overlap) to perform overall NSAA score regression</t>
+  </si>
+  <si>
+    <t>Stat values from NSAA\AD w/ seq_len=3 (w/ scaling seq_overlap) to perform overall NSAA score regression</t>
+  </si>
+  <si>
+    <t>Mean Squared Error = 0.0458, Mean Absolute Error = 0.1516, Root Mean Squared Error = 0.2139, R^2 Score = 0.999</t>
+  </si>
+  <si>
+    <t>X shape = (13265, 7, 30)</t>
+  </si>
+  <si>
+    <t>Y shape = (13265,)</t>
+  </si>
+  <si>
+    <t>Sequence length = 7</t>
+  </si>
+  <si>
+    <t>Mean Squared Error = 0.1063, Mean Absolute Error = 0.1993, Root Mean Squared Error = 0.326, R^2 Score = 0.9975</t>
+  </si>
+  <si>
+    <t>X shape = (13305, 5, 30)</t>
+  </si>
+  <si>
+    <t>Y shape = (13305,)</t>
+  </si>
+  <si>
+    <t>Sequence length = 5</t>
+  </si>
+  <si>
+    <t>Mean Squared Error = 0.124, Mean Absolute Error = 0.1937, Root Mean Squared Error = 0.3522, R^2 Score = 0.9972</t>
+  </si>
+  <si>
+    <t>X shape = (13453, 3, 30)</t>
+  </si>
+  <si>
+    <t>Y shape = (13453,)</t>
+  </si>
+  <si>
+    <t>Sequence length = 3</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA jointAngle all overall --seq_len=90 --seq_overlap=0.333 --discard_prop=0.333</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA jointAngle all overall --seq_len=120 --seq_overlap=0.5 --discard_prop=0.5</t>
+  </si>
+  <si>
+    <t>Mean Squared Error = 3.3633, Mean Absolute Error = 1.2131, Root Mean Squared Error = 1.8339, R^2 Score = 0.9257</t>
+  </si>
+  <si>
+    <t>X shape = (13314, 60, 66)</t>
+  </si>
+  <si>
+    <t>Mean Squared Error = 3.4289, Mean Absolute Error = 1.1326, Root Mean Squared Error = 1.8517, R^2 Score = 0.9261</t>
+  </si>
+  <si>
+    <t>X shape = (13315, 60, 66)</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA jointAngle all overall --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA jointAngle all overall --seq_len=180 --seq_overlap=0.667 --discard_prop=0.667</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA jointAngle all overall --seq_len=300 --seq_overlap=0.8 --discard_prop=0.8</t>
+  </si>
+  <si>
+    <t>Mean Squared Error = 3.1308, Mean Absolute Error = 1.0699, Root Mean Squared Error = 1.7694, R^2 Score = 0.9326</t>
+  </si>
+  <si>
+    <t>X shape = (13313, 60, 66)</t>
+  </si>
+  <si>
+    <t>Mean Squared Error = 2.4002, Mean Absolute Error = 0.8787, Root Mean Squared Error = 1.5493, R^2 Score = 0.9466</t>
+  </si>
+  <si>
+    <t>X shape = (13240, 60, 66)</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA jointAngle all overall --seq_len=1200 --seq_overlap=0.95 --discard_prop=0.95</t>
+  </si>
+  <si>
+    <t>Mean Squared Error = 1.0565, Mean Absolute Error = 0.5997, Root Mean Squared Error = 1.0279, R^2 Score = 0.9767</t>
+  </si>
+  <si>
+    <t>X shape = (13051, 60, 66)</t>
+  </si>
+  <si>
+    <t>Y shape = (13051,)</t>
+  </si>
+  <si>
+    <t>Mean Squared Error = 1.4799, Mean Absolute Error = 0.657, Root Mean Squared Error = 1.2165, R^2 Score = 0.967</t>
+  </si>
+  <si>
+    <t>X shape = (12436, 60, 66)</t>
+  </si>
+  <si>
+    <t>Y shape = (12436,)</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA jointAngle all overall --seq_len=2400 --seq_overlap=0.975 --discard_prop=0.975</t>
+  </si>
+  <si>
+    <t>Raw jointAngle values from NSAA\AD to perform overall NSAA score regression w/ 50% more sequence length w/ corresponding overlap (no discard_prop)</t>
+  </si>
+  <si>
+    <t>Raw jointAngle values from NSAA\AD to perform overall NSAA score regression w/ 100% more sequence length w/ corresponding overlap (no discard_prop)</t>
+  </si>
+  <si>
+    <t>Raw jointAngle values from NSAA\AD to perform overall NSAA score regression w/ 200% more sequence length w/ corresponding overlap (no discard_prop)</t>
+  </si>
+  <si>
+    <t>Raw jointAngle values from NSAA\AD to perform overall NSAA score regression w/ 50% more sequence length w/ corresponding overlap w/ corresponding discard_prop</t>
+  </si>
+  <si>
+    <t>Raw jointAngle values from NSAA\AD to perform overall NSAA score regression w/ 100% more sequence length w/ corresponding overlap w/ corresponding discard_prop</t>
+  </si>
+  <si>
+    <t>Raw jointAngle values from NSAA\AD to perform overall NSAA score regression w/ 200% more sequence length w/ corresponding overlap w/ corresponding discard_prop</t>
+  </si>
+  <si>
+    <t>Raw jointAngle values from NSAA\AD to perform overall NSAA score regression w/ 400% more sequence length w/ corresponding overlap w/ corresponding discard_prop</t>
+  </si>
+  <si>
+    <t>Raw jointAngle values from NSAA\AD to perform overall NSAA score regression w/ 900% more sequence length w/ corresponding overlap w/ corresponding discard_prop</t>
+  </si>
+  <si>
+    <t>Raw jointAngle values from NSAA\AD to perform overall NSAA score regression w/ 1900% more sequence length w/ corresponding overlap w/ corresponding discard_prop</t>
+  </si>
+  <si>
+    <t>Raw jointAngle values from NSAA\AD to perform overall NSAA score regression w/ 3900% more sequence length w/ corresponding overlap w/ corresponding discard_prop</t>
+  </si>
+  <si>
+    <t>Mean Squared Error = 0.3534, Mean Absolute Error = 0.406, Root Mean Squared Error = 0.5945, R^2 Score = 0.9917</t>
+  </si>
+  <si>
+    <t>X shape = (11530, 60, 66)</t>
+  </si>
+  <si>
+    <t>Y shape = (11530,)</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA jointAngle all overall --seq_len=4800 --seq_overlap=0.9875 --discard_prop=0.9875</t>
+  </si>
+  <si>
+    <t>Raw jointAngle values from NSAA\AD to perform overall NSAA score regression w/ 7900% more sequence length w/ corresponding overlap w/ corresponding discard_prop</t>
+  </si>
+  <si>
+    <t>Mean Squared Error = 0.3486, Mean Absolute Error = 0.4562, Root Mean Squared Error = 0.5905, R^2 Score = 0.9926</t>
+  </si>
+  <si>
+    <t>X shape = (10130, 60, 66)</t>
+  </si>
+  <si>
+    <t>Y shape = (10130,)</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA jointAngle all overall --seq_len=9600 --seq_overlap=0.99375 --discard_prop=0.99375</t>
+  </si>
+  <si>
+    <t>Raw jointAngle values from NSAA\AD to perform overall NSAA score regression w/ 15900% more sequence length w/ corresponding overlap w/ corresponding discard_prop</t>
+  </si>
+  <si>
+    <t>Mean Squared Error = 0.7334, Mean Absolute Error = 0.6984, Root Mean Squared Error = 0.8564, R^2 Score = 0.9803</t>
+  </si>
+  <si>
+    <t>X shape = (7481, 60, 66)</t>
+  </si>
+  <si>
+    <t>Y shape = (7481,)</t>
   </si>
 </sst>
 </file>
@@ -1413,10 +1599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9434AE6E-DEC1-4F2B-94BC-7DD094833B2C}">
-  <dimension ref="A1:P98"/>
+  <dimension ref="A1:P115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B65" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="H13" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5279,28 +5465,822 @@
       <c r="B83">
         <v>82</v>
       </c>
+      <c r="C83" t="s">
+        <v>341</v>
+      </c>
+      <c r="D83" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" t="s">
+        <v>10</v>
+      </c>
+      <c r="F83" t="s">
+        <v>287</v>
+      </c>
+      <c r="G83" t="s">
+        <v>288</v>
+      </c>
+      <c r="H83" t="s">
+        <v>289</v>
+      </c>
+      <c r="I83" t="s">
+        <v>290</v>
+      </c>
+      <c r="J83" t="s">
+        <v>15</v>
+      </c>
+      <c r="K83" t="s">
+        <v>16</v>
+      </c>
+      <c r="L83" t="s">
+        <v>17</v>
+      </c>
+      <c r="M83" t="s">
+        <v>18</v>
+      </c>
+      <c r="N83" t="s">
+        <v>19</v>
+      </c>
+      <c r="O83" t="s">
+        <v>20</v>
+      </c>
+      <c r="P83" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="84" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B84">
+        <v>83</v>
+      </c>
+      <c r="C84" t="s">
+        <v>347</v>
+      </c>
+      <c r="D84" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" t="s">
+        <v>10</v>
+      </c>
+      <c r="F84" t="s">
+        <v>344</v>
+      </c>
+      <c r="G84" t="s">
+        <v>350</v>
+      </c>
+      <c r="H84" t="s">
+        <v>351</v>
+      </c>
+      <c r="I84" t="s">
+        <v>352</v>
+      </c>
+      <c r="J84" t="s">
+        <v>15</v>
+      </c>
+      <c r="K84" t="s">
+        <v>353</v>
+      </c>
+      <c r="L84" t="s">
+        <v>17</v>
+      </c>
+      <c r="M84" t="s">
+        <v>18</v>
+      </c>
+      <c r="N84" t="s">
+        <v>19</v>
+      </c>
+      <c r="O84" t="s">
+        <v>20</v>
+      </c>
+      <c r="P84" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="85" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B85">
+        <v>84</v>
+      </c>
+      <c r="C85" t="s">
+        <v>348</v>
+      </c>
+      <c r="D85" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" t="s">
+        <v>10</v>
+      </c>
+      <c r="F85" t="s">
+        <v>346</v>
+      </c>
+      <c r="G85" t="s">
+        <v>354</v>
+      </c>
+      <c r="H85" t="s">
+        <v>355</v>
+      </c>
+      <c r="I85" t="s">
+        <v>356</v>
+      </c>
+      <c r="J85" t="s">
+        <v>15</v>
+      </c>
+      <c r="K85" t="s">
+        <v>357</v>
+      </c>
+      <c r="L85" t="s">
+        <v>17</v>
+      </c>
+      <c r="M85" t="s">
+        <v>18</v>
+      </c>
+      <c r="N85" t="s">
+        <v>19</v>
+      </c>
+      <c r="O85" t="s">
+        <v>20</v>
+      </c>
+      <c r="P85" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="86" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B86">
+        <v>85</v>
+      </c>
+      <c r="C86" t="s">
+        <v>349</v>
+      </c>
+      <c r="D86" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" t="s">
+        <v>10</v>
+      </c>
+      <c r="F86" t="s">
+        <v>345</v>
+      </c>
+      <c r="G86" t="s">
+        <v>358</v>
+      </c>
+      <c r="H86" t="s">
+        <v>359</v>
+      </c>
+      <c r="I86" t="s">
+        <v>360</v>
+      </c>
+      <c r="J86" t="s">
+        <v>15</v>
+      </c>
+      <c r="K86" t="s">
+        <v>361</v>
+      </c>
+      <c r="L86" t="s">
+        <v>17</v>
+      </c>
+      <c r="M86" t="s">
+        <v>18</v>
+      </c>
+      <c r="N86" t="s">
+        <v>19</v>
+      </c>
+      <c r="O86" t="s">
+        <v>20</v>
+      </c>
+      <c r="P86" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="87" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B87">
+        <v>86</v>
+      </c>
+      <c r="C87" t="s">
+        <v>242</v>
+      </c>
+      <c r="D87" t="s">
+        <v>75</v>
+      </c>
+      <c r="E87" t="s">
+        <v>27</v>
+      </c>
+      <c r="F87" t="s">
+        <v>152</v>
+      </c>
+      <c r="G87" t="s">
+        <v>243</v>
+      </c>
+      <c r="H87" t="s">
+        <v>244</v>
+      </c>
+      <c r="I87" t="s">
+        <v>223</v>
+      </c>
+      <c r="J87" t="s">
+        <v>15</v>
+      </c>
+      <c r="K87" t="s">
+        <v>32</v>
+      </c>
+      <c r="L87" t="s">
+        <v>33</v>
+      </c>
+      <c r="M87" t="s">
+        <v>34</v>
+      </c>
+      <c r="N87" t="s">
+        <v>19</v>
+      </c>
+      <c r="O87" t="s">
+        <v>20</v>
+      </c>
+      <c r="P87" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="88" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B88">
+        <v>87</v>
+      </c>
+      <c r="C88" t="s">
+        <v>383</v>
+      </c>
+      <c r="D88" t="s">
+        <v>75</v>
+      </c>
+      <c r="E88" t="s">
+        <v>27</v>
+      </c>
+      <c r="F88" t="s">
+        <v>246</v>
+      </c>
+      <c r="G88" t="s">
+        <v>247</v>
+      </c>
+      <c r="H88" t="s">
+        <v>248</v>
+      </c>
+      <c r="I88" t="s">
+        <v>228</v>
+      </c>
+      <c r="J88" t="s">
+        <v>15</v>
+      </c>
+      <c r="K88" t="s">
+        <v>229</v>
+      </c>
+      <c r="L88" t="s">
+        <v>33</v>
+      </c>
+      <c r="M88" t="s">
+        <v>34</v>
+      </c>
+      <c r="N88" t="s">
+        <v>19</v>
+      </c>
+      <c r="O88" t="s">
+        <v>20</v>
+      </c>
+      <c r="P88" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="89" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B89">
+        <v>88</v>
+      </c>
+      <c r="C89" t="s">
+        <v>384</v>
+      </c>
+      <c r="D89" t="s">
+        <v>75</v>
+      </c>
+      <c r="E89" t="s">
+        <v>27</v>
+      </c>
+      <c r="F89" t="s">
+        <v>250</v>
+      </c>
+      <c r="G89" t="s">
+        <v>251</v>
+      </c>
+      <c r="H89" t="s">
+        <v>252</v>
+      </c>
+      <c r="I89" t="s">
+        <v>234</v>
+      </c>
+      <c r="J89" t="s">
+        <v>15</v>
+      </c>
+      <c r="K89" t="s">
+        <v>235</v>
+      </c>
+      <c r="L89" t="s">
+        <v>33</v>
+      </c>
+      <c r="M89" t="s">
+        <v>34</v>
+      </c>
+      <c r="N89" t="s">
+        <v>19</v>
+      </c>
+      <c r="O89" t="s">
+        <v>20</v>
+      </c>
+      <c r="P89" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="90" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B90">
+        <v>89</v>
+      </c>
       <c r="C90" t="s">
+        <v>385</v>
+      </c>
+      <c r="D90" t="s">
+        <v>75</v>
+      </c>
+      <c r="E90" t="s">
+        <v>27</v>
+      </c>
+      <c r="F90" t="s">
+        <v>254</v>
+      </c>
+      <c r="G90" t="s">
+        <v>255</v>
+      </c>
+      <c r="H90" t="s">
+        <v>256</v>
+      </c>
+      <c r="I90" t="s">
+        <v>240</v>
+      </c>
+      <c r="J90" t="s">
+        <v>15</v>
+      </c>
+      <c r="K90" t="s">
+        <v>241</v>
+      </c>
+      <c r="L90" t="s">
+        <v>33</v>
+      </c>
+      <c r="M90" t="s">
+        <v>34</v>
+      </c>
+      <c r="N90" t="s">
+        <v>19</v>
+      </c>
+      <c r="O90" t="s">
+        <v>20</v>
+      </c>
+      <c r="P90" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="91" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B91">
+        <v>90</v>
+      </c>
+      <c r="C91" t="s">
+        <v>386</v>
+      </c>
+      <c r="D91" t="s">
+        <v>75</v>
+      </c>
+      <c r="E91" t="s">
+        <v>27</v>
+      </c>
+      <c r="F91" t="s">
+        <v>362</v>
+      </c>
+      <c r="G91" t="s">
+        <v>364</v>
+      </c>
+      <c r="H91" t="s">
+        <v>365</v>
+      </c>
+      <c r="I91" t="s">
+        <v>228</v>
+      </c>
+      <c r="J91" t="s">
+        <v>15</v>
+      </c>
+      <c r="K91" t="s">
+        <v>32</v>
+      </c>
+      <c r="L91" t="s">
+        <v>33</v>
+      </c>
+      <c r="M91" t="s">
+        <v>34</v>
+      </c>
+      <c r="N91" t="s">
+        <v>19</v>
+      </c>
+      <c r="O91" t="s">
+        <v>20</v>
+      </c>
+      <c r="P91" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="92" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B92">
+        <v>91</v>
+      </c>
+      <c r="C92" t="s">
+        <v>387</v>
+      </c>
+      <c r="D92" t="s">
+        <v>75</v>
+      </c>
+      <c r="E92" t="s">
+        <v>27</v>
+      </c>
+      <c r="F92" t="s">
+        <v>363</v>
+      </c>
+      <c r="G92" t="s">
+        <v>366</v>
+      </c>
+      <c r="H92" t="s">
+        <v>367</v>
+      </c>
+      <c r="I92" t="s">
+        <v>234</v>
+      </c>
+      <c r="J92" t="s">
+        <v>15</v>
+      </c>
+      <c r="K92" t="s">
+        <v>32</v>
+      </c>
+      <c r="L92" t="s">
+        <v>33</v>
+      </c>
+      <c r="M92" t="s">
+        <v>34</v>
+      </c>
+      <c r="N92" t="s">
+        <v>19</v>
+      </c>
+      <c r="O92" t="s">
+        <v>20</v>
+      </c>
+      <c r="P92" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="93" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B93">
+        <v>92</v>
+      </c>
+      <c r="C93" t="s">
+        <v>388</v>
+      </c>
+      <c r="D93" t="s">
+        <v>75</v>
+      </c>
+      <c r="E93" t="s">
+        <v>27</v>
+      </c>
+      <c r="F93" t="s">
+        <v>369</v>
+      </c>
+      <c r="G93" t="s">
+        <v>371</v>
+      </c>
+      <c r="H93" t="s">
+        <v>372</v>
+      </c>
+      <c r="I93" t="s">
+        <v>240</v>
+      </c>
+      <c r="J93" t="s">
+        <v>15</v>
+      </c>
+      <c r="K93" t="s">
+        <v>32</v>
+      </c>
+      <c r="L93" t="s">
+        <v>33</v>
+      </c>
+      <c r="M93" t="s">
+        <v>34</v>
+      </c>
+      <c r="N93" t="s">
+        <v>19</v>
+      </c>
+      <c r="O93" t="s">
+        <v>20</v>
+      </c>
+      <c r="P93" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="94" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B94">
+        <v>93</v>
+      </c>
+      <c r="C94" t="s">
+        <v>389</v>
+      </c>
+      <c r="D94" t="s">
+        <v>75</v>
+      </c>
+      <c r="E94" t="s">
+        <v>27</v>
+      </c>
+      <c r="F94" t="s">
+        <v>370</v>
+      </c>
+      <c r="G94" t="s">
+        <v>373</v>
+      </c>
+      <c r="H94" t="s">
+        <v>374</v>
+      </c>
+      <c r="I94" t="s">
+        <v>290</v>
+      </c>
+      <c r="J94" t="s">
+        <v>15</v>
+      </c>
+      <c r="K94" t="s">
+        <v>32</v>
+      </c>
+      <c r="L94" t="s">
+        <v>33</v>
+      </c>
+      <c r="M94" t="s">
+        <v>34</v>
+      </c>
+      <c r="N94" t="s">
+        <v>19</v>
+      </c>
+      <c r="O94" t="s">
+        <v>20</v>
+      </c>
+      <c r="P94" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="95" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B95">
+        <v>94</v>
+      </c>
+      <c r="C95" t="s">
+        <v>390</v>
+      </c>
+      <c r="D95" t="s">
+        <v>75</v>
+      </c>
+      <c r="E95" t="s">
+        <v>27</v>
+      </c>
+      <c r="F95" t="s">
+        <v>368</v>
+      </c>
+      <c r="G95" t="s">
+        <v>376</v>
+      </c>
+      <c r="H95" t="s">
+        <v>377</v>
+      </c>
+      <c r="I95" t="s">
+        <v>378</v>
+      </c>
+      <c r="J95" t="s">
+        <v>15</v>
+      </c>
+      <c r="K95" t="s">
+        <v>32</v>
+      </c>
+      <c r="L95" t="s">
+        <v>33</v>
+      </c>
+      <c r="M95" t="s">
+        <v>34</v>
+      </c>
+      <c r="N95" t="s">
+        <v>19</v>
+      </c>
+      <c r="O95" t="s">
+        <v>20</v>
+      </c>
+      <c r="P95" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="96" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B96">
+        <v>95</v>
+      </c>
+      <c r="C96" t="s">
+        <v>391</v>
+      </c>
+      <c r="D96" t="s">
+        <v>75</v>
+      </c>
+      <c r="E96" t="s">
+        <v>27</v>
+      </c>
+      <c r="F96" t="s">
+        <v>375</v>
+      </c>
+      <c r="G96" t="s">
+        <v>379</v>
+      </c>
+      <c r="H96" t="s">
+        <v>380</v>
+      </c>
+      <c r="I96" t="s">
+        <v>381</v>
+      </c>
+      <c r="J96" t="s">
+        <v>15</v>
+      </c>
+      <c r="K96" t="s">
+        <v>32</v>
+      </c>
+      <c r="L96" t="s">
+        <v>33</v>
+      </c>
+      <c r="M96" t="s">
+        <v>34</v>
+      </c>
+      <c r="N96" t="s">
+        <v>19</v>
+      </c>
+      <c r="O96" t="s">
+        <v>20</v>
+      </c>
+      <c r="P96" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="97" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B97">
+        <v>96</v>
+      </c>
+      <c r="C97" t="s">
+        <v>392</v>
+      </c>
+      <c r="D97" t="s">
+        <v>75</v>
+      </c>
+      <c r="E97" t="s">
+        <v>27</v>
+      </c>
+      <c r="F97" t="s">
+        <v>382</v>
+      </c>
+      <c r="G97" t="s">
+        <v>393</v>
+      </c>
+      <c r="H97" t="s">
+        <v>394</v>
+      </c>
+      <c r="I97" t="s">
+        <v>395</v>
+      </c>
+      <c r="J97" t="s">
+        <v>15</v>
+      </c>
+      <c r="K97" t="s">
+        <v>32</v>
+      </c>
+      <c r="L97" t="s">
+        <v>33</v>
+      </c>
+      <c r="M97" t="s">
+        <v>34</v>
+      </c>
+      <c r="N97" t="s">
+        <v>19</v>
+      </c>
+      <c r="O97" t="s">
+        <v>20</v>
+      </c>
+      <c r="P97" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="98" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B98">
+        <v>97</v>
+      </c>
+      <c r="C98" t="s">
+        <v>397</v>
+      </c>
+      <c r="D98" t="s">
+        <v>75</v>
+      </c>
+      <c r="E98" t="s">
+        <v>27</v>
+      </c>
+      <c r="F98" t="s">
+        <v>396</v>
+      </c>
+      <c r="G98" t="s">
+        <v>398</v>
+      </c>
+      <c r="H98" t="s">
+        <v>399</v>
+      </c>
+      <c r="I98" t="s">
+        <v>400</v>
+      </c>
+      <c r="J98" t="s">
+        <v>15</v>
+      </c>
+      <c r="K98" t="s">
+        <v>32</v>
+      </c>
+      <c r="L98" t="s">
+        <v>33</v>
+      </c>
+      <c r="M98" t="s">
+        <v>34</v>
+      </c>
+      <c r="N98" t="s">
+        <v>19</v>
+      </c>
+      <c r="O98" t="s">
+        <v>20</v>
+      </c>
+      <c r="P98" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="99" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B99">
+        <v>98</v>
+      </c>
+      <c r="C99" t="s">
+        <v>402</v>
+      </c>
+      <c r="D99" t="s">
+        <v>75</v>
+      </c>
+      <c r="E99" t="s">
+        <v>27</v>
+      </c>
+      <c r="F99" t="s">
+        <v>401</v>
+      </c>
+      <c r="G99" t="s">
+        <v>403</v>
+      </c>
+      <c r="H99" t="s">
+        <v>404</v>
+      </c>
+      <c r="I99" t="s">
+        <v>405</v>
+      </c>
+      <c r="J99" t="s">
+        <v>15</v>
+      </c>
+      <c r="K99" t="s">
+        <v>32</v>
+      </c>
+      <c r="L99" t="s">
+        <v>33</v>
+      </c>
+      <c r="M99" t="s">
+        <v>34</v>
+      </c>
+      <c r="N99" t="s">
+        <v>19</v>
+      </c>
+      <c r="O99" t="s">
+        <v>20</v>
+      </c>
+      <c r="P99" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="107" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="C107" t="s">
         <v>342</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D107" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="96" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="C96" t="s">
+    <row r="113" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C113" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="98" spans="3:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C98" t="s">
+    <row r="115" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C115" t="s">
         <v>284</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D115" t="s">
         <v>285</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E115" t="s">
         <v>286</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed issue with with setup rows in .mat files not being removed in ext_raw_measures.py, carried out more experiments and added to results, and added several batch files.
</commit_message>
<xml_diff>
--- a/project_files/documentation/RNN Results.xlsx
+++ b/project_files/documentation/RNN Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dheat\Dropbox\Imperial\Individual Project\indiv_proj\project_files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E39A13-1CFE-4536-9BE1-6AD7EE21191E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46983925-E199-4321-A0C7-DD631072538E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8778" xr2:uid="{F111C118-2C3B-40EB-A3AA-5A6786E31AB7}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="440">
   <si>
     <t>Notes</t>
   </si>
@@ -1248,16 +1248,125 @@
   </si>
   <si>
     <t>Y shape = (7481,)</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA jointAngle all dhc --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA jointAngle all acts --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA position all dhc --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA position all overall --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA position all acts --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA sensorMagneticField all dhc --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA sensorMagneticField all overall --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA sensorMagneticField all acts --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA jointAngleXZY all dhc --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA jointAngleXZY all overall --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA jointAngleXZY all acts --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA AD all overall --seq_len=10 --seq_overlap=0.9 --epochs=300</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA AD all dhc --seq_len=10 --seq_overlap=0.9 --epochs=300</t>
+  </si>
+  <si>
+    <t>python rnn.py NSAA AD all acts --seq_len=10 --seq_overlap=0.9 --epochs=300</t>
+  </si>
+  <si>
+    <t>python rnn.py 6minwalk-matfiles position all dhc --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9 --other_dir=6MW-matFiles</t>
+  </si>
+  <si>
+    <t>python ext_raw_measures.py 6minwalk-matfiles all all</t>
+  </si>
+  <si>
+    <t>python ext_raw_measures.py 6MW-matFiles all all</t>
+  </si>
+  <si>
+    <t>python comp_stat_vals.py 6MW-matFiles AD all --split_size=1</t>
+  </si>
+  <si>
+    <t>python rnn.py 6minwalk-matfiles position all overall --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9 --other_dir=6MW-matFiles</t>
+  </si>
+  <si>
+    <t>python rnn.py 6minwalk-matfiles position all acts --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9 --other_dir=6MW-matFiles</t>
+  </si>
+  <si>
+    <t>python rnn.py 6minwalk-matfiles sensorMagneticField all dhc --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9 --other_dir=6MW-matFiles</t>
+  </si>
+  <si>
+    <t>python rnn.py 6minwalk-matfiles sensorMagneticField all overall --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9 --other_dir=6MW-matFiles</t>
+  </si>
+  <si>
+    <t>python rnn.py 6minwalk-matfiles sensorMagneticField all acts --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9 --other_dir=6MW-matFiles</t>
+  </si>
+  <si>
+    <t>python rnn.py 6minwalk-matfiles jointAngle all dhc --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9 --other_dir=6MW-matFiles</t>
+  </si>
+  <si>
+    <t>python rnn.py 6minwalk-matfiles jointAngle all overall --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9 --other_dir=6MW-matFiles</t>
+  </si>
+  <si>
+    <t>python rnn.py 6minwalk-matfiles jointAngle all acts --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9 --other_dir=6MW-matFiles</t>
+  </si>
+  <si>
+    <t>python rnn.py 6minwalk-matfiles jointAngleXZY all dhc --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9 --other_dir=6MW-matFiles</t>
+  </si>
+  <si>
+    <t>python rnn.py 6minwalk-matfiles jointAngleXZY all overall --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9 --other_dir=6MW-matFiles</t>
+  </si>
+  <si>
+    <t>python rnn.py 6minwalk-matfiles jointAngleXZY all acts --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9 --other_dir=6MW-matFiles</t>
+  </si>
+  <si>
+    <t>python rnn.py 6minwalk-matfiles AD all dhc --seq_len=10 --seq_overlap=0.9 --epochs=300 --other_dir=6MW-matFiles</t>
+  </si>
+  <si>
+    <t>python rnn.py 6minwalk-matfiles AD all acts --seq_len=10 --seq_overlap=0.9 --epochs=300 --other_dir=6MW-matFiles</t>
+  </si>
+  <si>
+    <t>python rnn.py 6minwalk-matfiles AD all overall --seq_len=10 --seq_overlap=0.9 --epochs=300 --other_dir=6MW-matFiles</t>
+  </si>
+  <si>
+    <t>python ft_sel_red.py 6MW-matFiles AD all pca --num_features=30 --no_normalize</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1283,8 +1392,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1599,10 +1711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9434AE6E-DEC1-4F2B-94BC-7DD094833B2C}">
-  <dimension ref="A1:P115"/>
+  <dimension ref="A1:P140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H13" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" topLeftCell="F115" workbookViewId="0">
+      <selection activeCell="H140" sqref="H140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6260,28 +6372,296 @@
         <v>21</v>
       </c>
     </row>
+    <row r="104" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F104" t="s">
+        <v>408</v>
+      </c>
+      <c r="G104" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="105" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F105" t="s">
+        <v>409</v>
+      </c>
+      <c r="G105" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="106" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F106" t="s">
+        <v>410</v>
+      </c>
+      <c r="G106" t="s">
+        <v>417</v>
+      </c>
+    </row>
     <row r="107" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="C107" t="s">
+      <c r="F107" t="s">
+        <v>411</v>
+      </c>
+      <c r="G107" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="108" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F108" t="s">
+        <v>412</v>
+      </c>
+      <c r="G108" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="109" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F109" t="s">
+        <v>413</v>
+      </c>
+      <c r="G109" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="110" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F110" t="s">
+        <v>406</v>
+      </c>
+      <c r="G110" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="111" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F111" t="s">
+        <v>368</v>
+      </c>
+      <c r="G111" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="112" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F112" t="s">
+        <v>407</v>
+      </c>
+      <c r="G112" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="113" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F113" t="s">
+        <v>414</v>
+      </c>
+      <c r="G113" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="114" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F114" t="s">
+        <v>415</v>
+      </c>
+      <c r="G114" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="115" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="C115" t="s">
         <v>342</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D115" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="113" spans="3:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C113" t="s">
+      <c r="F115" t="s">
+        <v>416</v>
+      </c>
+      <c r="G115" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="116" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F116" t="s">
+        <v>419</v>
+      </c>
+      <c r="G116" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="117" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F117" t="s">
+        <v>418</v>
+      </c>
+      <c r="G117" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="118" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F118" t="s">
+        <v>420</v>
+      </c>
+      <c r="G118" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="121" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="C121" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="115" spans="3:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C115" t="s">
+    <row r="122" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F122" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G122" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="123" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="C123" t="s">
         <v>284</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D123" t="s">
         <v>285</v>
       </c>
-      <c r="E115" t="s">
+      <c r="E123" t="s">
         <v>286</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="G123" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="124" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F124" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="G124" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="125" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F125" t="s">
+        <v>421</v>
+      </c>
+      <c r="G125" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="126" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F126" t="s">
+        <v>425</v>
+      </c>
+      <c r="G126" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="127" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F127" t="s">
+        <v>426</v>
+      </c>
+      <c r="G127" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="128" spans="3:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F128" t="s">
+        <v>427</v>
+      </c>
+      <c r="G128" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="129" spans="6:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F129" t="s">
+        <v>428</v>
+      </c>
+      <c r="G129" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="130" spans="6:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F130" t="s">
+        <v>429</v>
+      </c>
+      <c r="G130" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="131" spans="6:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F131" t="s">
+        <v>430</v>
+      </c>
+      <c r="G131" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="132" spans="6:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F132" t="s">
+        <v>431</v>
+      </c>
+      <c r="G132" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="133" spans="6:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F133" t="s">
+        <v>432</v>
+      </c>
+      <c r="G133" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="134" spans="6:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F134" t="s">
+        <v>433</v>
+      </c>
+      <c r="G134" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="135" spans="6:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F135" t="s">
+        <v>434</v>
+      </c>
+      <c r="G135" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="136" spans="6:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F136" t="s">
+        <v>435</v>
+      </c>
+      <c r="G136" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="137" spans="6:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F137" t="s">
+        <v>439</v>
+      </c>
+      <c r="G137" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="138" spans="6:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F138" t="s">
+        <v>436</v>
+      </c>
+      <c r="G138" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="139" spans="6:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F139" t="s">
+        <v>438</v>
+      </c>
+      <c r="G139" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="140" spans="6:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F140" t="s">
+        <v>437</v>
+      </c>
+      <c r="G140" t="s">
+        <v>417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'test_altdirs.py' script, modified 'graph_creator.py' and 'model_predictor.py' to correctly work with it, and relocated .cmd scripts.
</commit_message>
<xml_diff>
--- a/project_files/documentation/RNN Results.xlsx
+++ b/project_files/documentation/RNN Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dheat\Dropbox\Imperial\Individual Project\indiv_proj\project_files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46983925-E199-4321-A0C7-DD631072538E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A451E527-C462-429F-898F-CF944F4B43E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8778" xr2:uid="{F111C118-2C3B-40EB-A3AA-5A6786E31AB7}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="438">
   <si>
     <t>Notes</t>
   </si>
@@ -1058,9 +1058,6 @@
     <t>Stat values from NSAA\AD w/ seq_len=10 (w/ scaling seq_overlap) to perform overall NSAA score regression</t>
   </si>
   <si>
-    <t>Raw joint angles from allmatfiles to perform overall NSAA score regression</t>
-  </si>
-  <si>
     <t>python ext_raw_measures.py allmatfiles all jointAngle</t>
   </si>
   <si>
@@ -1281,9 +1278,6 @@
   </si>
   <si>
     <t>python rnn.py NSAA jointAngleXZY all acts --seq_len=600 --seq_overlap=0.9 --discard_prop=0.9</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>python rnn.py NSAA AD all overall --seq_len=10 --seq_overlap=0.9 --epochs=300</t>
@@ -1711,10 +1705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9434AE6E-DEC1-4F2B-94BC-7DD094833B2C}">
-  <dimension ref="A1:P140"/>
+  <dimension ref="A1:P154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F115" workbookViewId="0">
-      <selection activeCell="H140" sqref="H140"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5625,7 +5619,7 @@
         <v>83</v>
       </c>
       <c r="C84" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D84" t="s">
         <v>9</v>
@@ -5634,22 +5628,22 @@
         <v>10</v>
       </c>
       <c r="F84" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G84" t="s">
+        <v>349</v>
+      </c>
+      <c r="H84" t="s">
         <v>350</v>
       </c>
-      <c r="H84" t="s">
+      <c r="I84" t="s">
         <v>351</v>
       </c>
-      <c r="I84" t="s">
+      <c r="J84" t="s">
+        <v>15</v>
+      </c>
+      <c r="K84" t="s">
         <v>352</v>
-      </c>
-      <c r="J84" t="s">
-        <v>15</v>
-      </c>
-      <c r="K84" t="s">
-        <v>353</v>
       </c>
       <c r="L84" t="s">
         <v>17</v>
@@ -5672,7 +5666,7 @@
         <v>84</v>
       </c>
       <c r="C85" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D85" t="s">
         <v>9</v>
@@ -5681,22 +5675,22 @@
         <v>10</v>
       </c>
       <c r="F85" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G85" t="s">
+        <v>353</v>
+      </c>
+      <c r="H85" t="s">
         <v>354</v>
       </c>
-      <c r="H85" t="s">
+      <c r="I85" t="s">
         <v>355</v>
       </c>
-      <c r="I85" t="s">
+      <c r="J85" t="s">
+        <v>15</v>
+      </c>
+      <c r="K85" t="s">
         <v>356</v>
-      </c>
-      <c r="J85" t="s">
-        <v>15</v>
-      </c>
-      <c r="K85" t="s">
-        <v>357</v>
       </c>
       <c r="L85" t="s">
         <v>17</v>
@@ -5719,7 +5713,7 @@
         <v>85</v>
       </c>
       <c r="C86" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D86" t="s">
         <v>9</v>
@@ -5728,22 +5722,22 @@
         <v>10</v>
       </c>
       <c r="F86" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G86" t="s">
+        <v>357</v>
+      </c>
+      <c r="H86" t="s">
         <v>358</v>
       </c>
-      <c r="H86" t="s">
+      <c r="I86" t="s">
         <v>359</v>
       </c>
-      <c r="I86" t="s">
+      <c r="J86" t="s">
+        <v>15</v>
+      </c>
+      <c r="K86" t="s">
         <v>360</v>
-      </c>
-      <c r="J86" t="s">
-        <v>15</v>
-      </c>
-      <c r="K86" t="s">
-        <v>361</v>
       </c>
       <c r="L86" t="s">
         <v>17</v>
@@ -5813,7 +5807,7 @@
         <v>87</v>
       </c>
       <c r="C88" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D88" t="s">
         <v>75</v>
@@ -5860,7 +5854,7 @@
         <v>88</v>
       </c>
       <c r="C89" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D89" t="s">
         <v>75</v>
@@ -5907,7 +5901,7 @@
         <v>89</v>
       </c>
       <c r="C90" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D90" t="s">
         <v>75</v>
@@ -5954,7 +5948,7 @@
         <v>90</v>
       </c>
       <c r="C91" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D91" t="s">
         <v>75</v>
@@ -5963,13 +5957,13 @@
         <v>27</v>
       </c>
       <c r="F91" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G91" t="s">
+        <v>363</v>
+      </c>
+      <c r="H91" t="s">
         <v>364</v>
-      </c>
-      <c r="H91" t="s">
-        <v>365</v>
       </c>
       <c r="I91" t="s">
         <v>228</v>
@@ -6001,7 +5995,7 @@
         <v>91</v>
       </c>
       <c r="C92" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D92" t="s">
         <v>75</v>
@@ -6010,13 +6004,13 @@
         <v>27</v>
       </c>
       <c r="F92" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G92" t="s">
+        <v>365</v>
+      </c>
+      <c r="H92" t="s">
         <v>366</v>
-      </c>
-      <c r="H92" t="s">
-        <v>367</v>
       </c>
       <c r="I92" t="s">
         <v>234</v>
@@ -6048,7 +6042,7 @@
         <v>92</v>
       </c>
       <c r="C93" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D93" t="s">
         <v>75</v>
@@ -6057,13 +6051,13 @@
         <v>27</v>
       </c>
       <c r="F93" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G93" t="s">
+        <v>370</v>
+      </c>
+      <c r="H93" t="s">
         <v>371</v>
-      </c>
-      <c r="H93" t="s">
-        <v>372</v>
       </c>
       <c r="I93" t="s">
         <v>240</v>
@@ -6095,7 +6089,7 @@
         <v>93</v>
       </c>
       <c r="C94" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D94" t="s">
         <v>75</v>
@@ -6104,13 +6098,13 @@
         <v>27</v>
       </c>
       <c r="F94" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G94" t="s">
+        <v>372</v>
+      </c>
+      <c r="H94" t="s">
         <v>373</v>
-      </c>
-      <c r="H94" t="s">
-        <v>374</v>
       </c>
       <c r="I94" t="s">
         <v>290</v>
@@ -6142,7 +6136,7 @@
         <v>94</v>
       </c>
       <c r="C95" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D95" t="s">
         <v>75</v>
@@ -6151,16 +6145,16 @@
         <v>27</v>
       </c>
       <c r="F95" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G95" t="s">
+        <v>375</v>
+      </c>
+      <c r="H95" t="s">
         <v>376</v>
       </c>
-      <c r="H95" t="s">
+      <c r="I95" t="s">
         <v>377</v>
-      </c>
-      <c r="I95" t="s">
-        <v>378</v>
       </c>
       <c r="J95" t="s">
         <v>15</v>
@@ -6189,7 +6183,7 @@
         <v>95</v>
       </c>
       <c r="C96" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D96" t="s">
         <v>75</v>
@@ -6198,16 +6192,16 @@
         <v>27</v>
       </c>
       <c r="F96" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G96" t="s">
+        <v>378</v>
+      </c>
+      <c r="H96" t="s">
         <v>379</v>
       </c>
-      <c r="H96" t="s">
+      <c r="I96" t="s">
         <v>380</v>
-      </c>
-      <c r="I96" t="s">
-        <v>381</v>
       </c>
       <c r="J96" t="s">
         <v>15</v>
@@ -6236,7 +6230,7 @@
         <v>96</v>
       </c>
       <c r="C97" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D97" t="s">
         <v>75</v>
@@ -6245,16 +6239,16 @@
         <v>27</v>
       </c>
       <c r="F97" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G97" t="s">
+        <v>392</v>
+      </c>
+      <c r="H97" t="s">
         <v>393</v>
       </c>
-      <c r="H97" t="s">
+      <c r="I97" t="s">
         <v>394</v>
-      </c>
-      <c r="I97" t="s">
-        <v>395</v>
       </c>
       <c r="J97" t="s">
         <v>15</v>
@@ -6283,7 +6277,7 @@
         <v>97</v>
       </c>
       <c r="C98" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D98" t="s">
         <v>75</v>
@@ -6292,16 +6286,16 @@
         <v>27</v>
       </c>
       <c r="F98" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G98" t="s">
+        <v>397</v>
+      </c>
+      <c r="H98" t="s">
         <v>398</v>
       </c>
-      <c r="H98" t="s">
+      <c r="I98" t="s">
         <v>399</v>
-      </c>
-      <c r="I98" t="s">
-        <v>400</v>
       </c>
       <c r="J98" t="s">
         <v>15</v>
@@ -6330,7 +6324,7 @@
         <v>98</v>
       </c>
       <c r="C99" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D99" t="s">
         <v>75</v>
@@ -6339,16 +6333,16 @@
         <v>27</v>
       </c>
       <c r="F99" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G99" t="s">
+        <v>402</v>
+      </c>
+      <c r="H99" t="s">
         <v>403</v>
       </c>
-      <c r="H99" t="s">
+      <c r="I99" t="s">
         <v>404</v>
-      </c>
-      <c r="I99" t="s">
-        <v>405</v>
       </c>
       <c r="J99" t="s">
         <v>15</v>
@@ -6372,296 +6366,396 @@
         <v>21</v>
       </c>
     </row>
+    <row r="100" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B100">
+        <v>99</v>
+      </c>
+      <c r="C100" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="101" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B101">
+        <v>100</v>
+      </c>
+      <c r="C101" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="102" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B102">
+        <v>101</v>
+      </c>
+      <c r="C102" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="103" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B103">
+        <v>102</v>
+      </c>
+      <c r="C103" t="s">
+        <v>410</v>
+      </c>
+    </row>
     <row r="104" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F104" t="s">
-        <v>408</v>
-      </c>
-      <c r="G104" t="s">
+      <c r="B104">
+        <v>103</v>
+      </c>
+      <c r="C104" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="105" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B105">
+        <v>104</v>
+      </c>
+      <c r="C105" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="106" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B106">
+        <v>105</v>
+      </c>
+      <c r="C106" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="107" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B107">
+        <v>106</v>
+      </c>
+      <c r="C107" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="108" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B108">
+        <v>107</v>
+      </c>
+      <c r="C108" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="109" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B109">
+        <v>108</v>
+      </c>
+      <c r="C109" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="110" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B110">
+        <v>109</v>
+      </c>
+      <c r="C110" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="111" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B111">
+        <v>110</v>
+      </c>
+      <c r="C111" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="112" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B112">
+        <v>111</v>
+      </c>
+      <c r="C112" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="105" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F105" t="s">
-        <v>409</v>
-      </c>
-      <c r="G105" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="106" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F106" t="s">
-        <v>410</v>
-      </c>
-      <c r="G106" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="107" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F107" t="s">
-        <v>411</v>
-      </c>
-      <c r="G107" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="108" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F108" t="s">
-        <v>412</v>
-      </c>
-      <c r="G108" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="109" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F109" t="s">
-        <v>413</v>
-      </c>
-      <c r="G109" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="110" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F110" t="s">
-        <v>406</v>
-      </c>
-      <c r="G110" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="111" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F111" t="s">
-        <v>368</v>
-      </c>
-      <c r="G111" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="112" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F112" t="s">
-        <v>407</v>
-      </c>
-      <c r="G112" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="113" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F113" t="s">
-        <v>414</v>
-      </c>
-      <c r="G113" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="114" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F114" t="s">
-        <v>415</v>
-      </c>
-      <c r="G114" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="115" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C115" t="s">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B113">
+        <v>112</v>
+      </c>
+      <c r="C113" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B114">
+        <v>113</v>
+      </c>
+      <c r="C114" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B115">
+        <v>114</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B116">
+        <v>115</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B117">
+        <v>116</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B118">
+        <v>117</v>
+      </c>
+      <c r="C118" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B119">
+        <v>118</v>
+      </c>
+      <c r="C119" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B120">
+        <v>119</v>
+      </c>
+      <c r="C120" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B121">
+        <v>120</v>
+      </c>
+      <c r="C121" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B122">
+        <v>121</v>
+      </c>
+      <c r="C122" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B123">
+        <v>122</v>
+      </c>
+      <c r="C123" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B124">
+        <v>123</v>
+      </c>
+      <c r="C124" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B125">
+        <v>124</v>
+      </c>
+      <c r="C125" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B126">
+        <v>125</v>
+      </c>
+      <c r="C126" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B127">
+        <v>126</v>
+      </c>
+      <c r="C127" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B128">
+        <v>127</v>
+      </c>
+      <c r="C128" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B129">
+        <v>128</v>
+      </c>
+      <c r="C129" t="s">
+        <v>433</v>
+      </c>
+      <c r="D129" t="s">
         <v>342</v>
       </c>
-      <c r="D115" t="s">
-        <v>343</v>
-      </c>
-      <c r="F115" t="s">
-        <v>416</v>
-      </c>
-      <c r="G115" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="116" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F116" t="s">
-        <v>419</v>
-      </c>
-      <c r="G116" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="117" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F117" t="s">
-        <v>418</v>
-      </c>
-      <c r="G117" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="118" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F118" t="s">
-        <v>420</v>
-      </c>
-      <c r="G118" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="121" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C121" t="s">
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B130">
+        <v>129</v>
+      </c>
+      <c r="C130" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B131">
+        <v>130</v>
+      </c>
+      <c r="C131" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B132">
+        <v>131</v>
+      </c>
+      <c r="C132" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B133">
+        <v>132</v>
+      </c>
+      <c r="C133" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B134">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B135">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B136">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B137">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B138">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B139">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B140">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B141">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B142">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B143">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B144">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B145">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B146">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B147">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B148">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B149">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B150">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B151">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B152">
+        <v>151</v>
+      </c>
+      <c r="C152" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="122" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F122" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="G122" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="123" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="C123" t="s">
+    <row r="153" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B153">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B154">
+        <v>153</v>
+      </c>
+      <c r="C154" t="s">
         <v>284</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D154" t="s">
         <v>285</v>
       </c>
-      <c r="E123" t="s">
+      <c r="E154" t="s">
         <v>286</v>
-      </c>
-      <c r="F123" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="G123" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="124" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F124" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="G124" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="125" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F125" t="s">
-        <v>421</v>
-      </c>
-      <c r="G125" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="126" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F126" t="s">
-        <v>425</v>
-      </c>
-      <c r="G126" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="127" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F127" t="s">
-        <v>426</v>
-      </c>
-      <c r="G127" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="128" spans="3:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F128" t="s">
-        <v>427</v>
-      </c>
-      <c r="G128" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="129" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F129" t="s">
-        <v>428</v>
-      </c>
-      <c r="G129" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="130" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F130" t="s">
-        <v>429</v>
-      </c>
-      <c r="G130" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="131" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F131" t="s">
-        <v>430</v>
-      </c>
-      <c r="G131" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="132" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F132" t="s">
-        <v>431</v>
-      </c>
-      <c r="G132" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="133" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F133" t="s">
-        <v>432</v>
-      </c>
-      <c r="G133" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="134" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F134" t="s">
-        <v>433</v>
-      </c>
-      <c r="G134" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="135" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F135" t="s">
-        <v>434</v>
-      </c>
-      <c r="G135" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="136" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F136" t="s">
-        <v>435</v>
-      </c>
-      <c r="G136" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="137" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F137" t="s">
-        <v>439</v>
-      </c>
-      <c r="G137" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="138" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F138" t="s">
-        <v>436</v>
-      </c>
-      <c r="G138" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="139" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F139" t="s">
-        <v>438</v>
-      </c>
-      <c r="G139" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="140" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F140" t="s">
-        <v>437</v>
-      </c>
-      <c r="G140" t="s">
-        <v>417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added several more script explanations, modified 'file_renamer', 'comp_stat_vals', and 'ft_sel_red' to work as pipeline with newly downloaded files, added more stat values outputs to come from 'graph_creator', fixed output writing functionality with 'model_predictor', and removed redundant params in 'rnn'.
</commit_message>
<xml_diff>
--- a/project_files/documentation/RNN Results.xlsx
+++ b/project_files/documentation/RNN Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dheat\Dropbox\Imperial\Individual Project\indiv_proj\project_files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A451E527-C462-429F-898F-CF944F4B43E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B02787-C89D-4906-B28A-CDEAC0BE0BE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8778" xr2:uid="{F111C118-2C3B-40EB-A3AA-5A6786E31AB7}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="448">
   <si>
     <t>Notes</t>
   </si>
@@ -1344,6 +1344,36 @@
   </si>
   <si>
     <t>python ft_sel_red.py 6MW-matFiles AD all pca --num_features=30 --no_normalize</t>
+  </si>
+  <si>
+    <t>Setup of all needed models (note that here ALL files are included in the dataset)</t>
+  </si>
+  <si>
+    <t>python test_altdirs.py allmatfiles NSAA_6minwalk-matfiles jointAngle</t>
+  </si>
+  <si>
+    <t>Testing all files in 'allmatfiles' on models trained on 'NSAA' and '6minwalk' files and record results in 'model_predictions'</t>
+  </si>
+  <si>
+    <t>python model_predictor.py NSAA AD,jointAngle,jointAngleXZY,position,sensorMagneticField D3</t>
+  </si>
+  <si>
+    <t>python model_predictor.py NSAA AD,jointAngle,jointAngleXZY,position,sensorMagneticField D3 --use_seen</t>
+  </si>
+  <si>
+    <t>python model_predictor.py NSAA AD D3</t>
+  </si>
+  <si>
+    <t>python model_predictor.py NSAA jointAngle D3</t>
+  </si>
+  <si>
+    <t>python model_predictor.py NSAA jointAngleXZY D3</t>
+  </si>
+  <si>
+    <t>python model_predictor.py NSAA position D3</t>
+  </si>
+  <si>
+    <t>python model_predictor.py NSAA sensorMagneticField D3</t>
   </si>
 </sst>
 </file>
@@ -1707,8 +1737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9434AE6E-DEC1-4F2B-94BC-7DD094833B2C}">
   <dimension ref="A1:P154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="D133" sqref="D133"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6225,7 +6255,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B97">
         <v>96</v>
       </c>
@@ -6272,7 +6302,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="98" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B98">
         <v>97</v>
       </c>
@@ -6319,7 +6349,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="99" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B99">
         <v>98</v>
       </c>
@@ -6366,7 +6396,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="100" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" t="s">
+        <v>438</v>
+      </c>
       <c r="B100">
         <v>99</v>
       </c>
@@ -6374,7 +6407,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="101" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B101">
         <v>100</v>
       </c>
@@ -6382,7 +6415,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="102" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B102">
         <v>101</v>
       </c>
@@ -6390,7 +6423,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="103" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B103">
         <v>102</v>
       </c>
@@ -6398,7 +6431,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="104" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B104">
         <v>103</v>
       </c>
@@ -6406,7 +6439,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="105" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B105">
         <v>104</v>
       </c>
@@ -6414,7 +6447,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="106" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B106">
         <v>105</v>
       </c>
@@ -6422,7 +6455,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="107" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B107">
         <v>106</v>
       </c>
@@ -6430,7 +6463,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="108" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B108">
         <v>107</v>
       </c>
@@ -6438,7 +6471,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="109" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B109">
         <v>108</v>
       </c>
@@ -6446,7 +6479,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="110" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B110">
         <v>109</v>
       </c>
@@ -6454,7 +6487,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="111" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B111">
         <v>110</v>
       </c>
@@ -6462,7 +6495,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="112" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B112">
         <v>111</v>
       </c>
@@ -6598,7 +6631,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B129">
         <v>128</v>
       </c>
@@ -6609,7 +6642,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B130">
         <v>129</v>
       </c>
@@ -6617,7 +6650,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B131">
         <v>130</v>
       </c>
@@ -6625,7 +6658,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B132">
         <v>131</v>
       </c>
@@ -6633,7 +6666,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B133">
         <v>132</v>
       </c>
@@ -6641,57 +6674,84 @@
         <v>435</v>
       </c>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134" t="s">
+        <v>440</v>
+      </c>
       <c r="B134">
         <v>133</v>
       </c>
-    </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C134" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B135">
         <v>134</v>
       </c>
-    </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C135" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B136">
         <v>135</v>
       </c>
-    </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C136" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B137">
         <v>136</v>
       </c>
-    </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C137" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B138">
         <v>137</v>
       </c>
-    </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C138" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B139">
         <v>138</v>
       </c>
-    </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C139" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B140">
         <v>139</v>
       </c>
-    </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C140" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B141">
         <v>140</v>
       </c>
-    </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C141" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B142">
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B143">
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B144">
         <v>143</v>
       </c>

</xml_diff>

<commit_message>
Modified 'source' files to work with 'left-out' directory files, added 'left-out' predictions to 'model_predictions.csv', added another script README, and added more to the experiments discussion.
</commit_message>
<xml_diff>
--- a/project_files/documentation/RNN Results.xlsx
+++ b/project_files/documentation/RNN Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dheat\Dropbox\Imperial\Individual Project\indiv_proj\project_files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B02787-C89D-4906-B28A-CDEAC0BE0BE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69EA756-FF1A-475F-AF2B-FB8B4EE7D792}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8778" xr2:uid="{F111C118-2C3B-40EB-A3AA-5A6786E31AB7}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{F111C118-2C3B-40EB-A3AA-5A6786E31AB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="452">
   <si>
     <t>Notes</t>
   </si>
@@ -1374,6 +1374,18 @@
   </si>
   <si>
     <t>python model_predictor.py NSAA sensorMagneticField D3</t>
+  </si>
+  <si>
+    <t>Setting up of 'left-out' dir files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python comp_stat_vals.py left-out AD all --split_size=1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">python ft_sel_red.py left-out AD all pca --num_features=30 --no_normalize </t>
+  </si>
+  <si>
+    <t>python ext_raw_measures.py left-out all all</t>
   </si>
 </sst>
 </file>
@@ -1737,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9434AE6E-DEC1-4F2B-94BC-7DD094833B2C}">
   <dimension ref="A1:P154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="C136" sqref="C136"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6631,7 +6643,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B129">
         <v>128</v>
       </c>
@@ -6642,7 +6654,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B130">
         <v>129</v>
       </c>
@@ -6650,7 +6662,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B131">
         <v>130</v>
       </c>
@@ -6658,7 +6670,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B132">
         <v>131</v>
       </c>
@@ -6666,7 +6678,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B133">
         <v>132</v>
       </c>
@@ -6674,7 +6686,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
         <v>440</v>
       </c>
@@ -6685,7 +6697,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B135">
         <v>134</v>
       </c>
@@ -6693,7 +6705,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B136">
         <v>135</v>
       </c>
@@ -6701,7 +6713,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B137">
         <v>136</v>
       </c>
@@ -6709,7 +6721,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B138">
         <v>137</v>
       </c>
@@ -6717,7 +6729,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B139">
         <v>138</v>
       </c>
@@ -6725,7 +6737,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B140">
         <v>139</v>
       </c>
@@ -6733,7 +6745,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B141">
         <v>140</v>
       </c>
@@ -6741,17 +6753,29 @@
         <v>447</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A142" t="s">
+        <v>448</v>
+      </c>
       <c r="B142">
         <v>141</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C142" t="s">
+        <v>449</v>
+      </c>
+      <c r="D142" t="s">
+        <v>450</v>
+      </c>
+      <c r="E142" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B143">
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B144">
         <v>143</v>
       </c>

</xml_diff>

<commit_message>
Added extensively to both 'Script Ecosystem Overview' and 'Experiments and Results Discussion', with minor modifications to the results files and refactoring to several 'source' files.
</commit_message>
<xml_diff>
--- a/project_files/documentation/RNN Results.xlsx
+++ b/project_files/documentation/RNN Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dheat\Dropbox\Imperial\Individual Project\indiv_proj\project_files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69EA756-FF1A-475F-AF2B-FB8B4EE7D792}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADD5286-A6A4-4F7E-AE5A-81479E090683}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{F111C118-2C3B-40EB-A3AA-5A6786E31AB7}"/>
   </bookViews>
@@ -1392,7 +1392,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1407,13 +1407,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1428,11 +1464,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1749,8 +1791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9434AE6E-DEC1-4F2B-94BC-7DD094833B2C}">
   <dimension ref="A1:P154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="C142" sqref="C142"/>
+    <sheetView tabSelected="1" topLeftCell="G79" workbookViewId="0">
+      <selection activeCell="G99" sqref="G99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4341,2070 +4383,2070 @@
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B56">
+      <c r="B56" s="2">
         <v>55</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F56" t="s">
+      <c r="E56" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G56" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="H56" t="s">
+      <c r="H56" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I56" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="J56" t="s">
-        <v>15</v>
-      </c>
-      <c r="K56" t="s">
+      <c r="J56" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K56" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L56" t="s">
+      <c r="L56" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="M56" t="s">
+      <c r="M56" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N56" t="s">
-        <v>19</v>
-      </c>
-      <c r="O56" t="s">
-        <v>20</v>
-      </c>
-      <c r="P56" t="s">
+      <c r="N56" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O56" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P56" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B57">
+      <c r="B57" s="2">
         <v>56</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E57" t="s">
-        <v>27</v>
-      </c>
-      <c r="F57" t="s">
+      <c r="E57" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G57" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="H57" t="s">
+      <c r="H57" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="I57" t="s">
+      <c r="I57" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="J57" t="s">
-        <v>15</v>
-      </c>
-      <c r="K57" t="s">
+      <c r="J57" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K57" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="L57" t="s">
+      <c r="L57" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="M57" t="s">
+      <c r="M57" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N57" t="s">
-        <v>19</v>
-      </c>
-      <c r="O57" t="s">
-        <v>20</v>
-      </c>
-      <c r="P57" t="s">
+      <c r="N57" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O57" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P57" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B58">
+      <c r="B58" s="2">
         <v>57</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E58" t="s">
-        <v>27</v>
-      </c>
-      <c r="F58" t="s">
+      <c r="E58" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G58" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="H58" t="s">
+      <c r="H58" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="I58" t="s">
+      <c r="I58" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="J58" t="s">
-        <v>15</v>
-      </c>
-      <c r="K58" t="s">
+      <c r="J58" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K58" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="L58" t="s">
+      <c r="L58" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="M58" t="s">
+      <c r="M58" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N58" t="s">
-        <v>19</v>
-      </c>
-      <c r="O58" t="s">
-        <v>20</v>
-      </c>
-      <c r="P58" t="s">
+      <c r="N58" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O58" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P58" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B59">
+      <c r="B59" s="2">
         <v>58</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E59" t="s">
-        <v>27</v>
-      </c>
-      <c r="F59" t="s">
+      <c r="E59" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F59" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G59" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H59" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="I59" t="s">
+      <c r="I59" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="J59" t="s">
-        <v>15</v>
-      </c>
-      <c r="K59" t="s">
+      <c r="J59" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K59" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="L59" t="s">
+      <c r="L59" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="M59" t="s">
+      <c r="M59" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N59" t="s">
-        <v>19</v>
-      </c>
-      <c r="O59" t="s">
-        <v>20</v>
-      </c>
-      <c r="P59" t="s">
+      <c r="N59" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O59" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P59" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B60">
+      <c r="B60" s="2">
         <v>59</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E60" t="s">
-        <v>27</v>
-      </c>
-      <c r="F60" t="s">
+      <c r="E60" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F60" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G60" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="H60" t="s">
+      <c r="H60" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="I60" t="s">
+      <c r="I60" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="J60" t="s">
-        <v>15</v>
-      </c>
-      <c r="K60" t="s">
+      <c r="J60" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K60" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L60" t="s">
+      <c r="L60" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M60" t="s">
+      <c r="M60" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N60" t="s">
-        <v>19</v>
-      </c>
-      <c r="O60" t="s">
-        <v>20</v>
-      </c>
-      <c r="P60" t="s">
+      <c r="N60" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P60" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B61">
+      <c r="B61" s="2">
         <v>60</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E61" t="s">
-        <v>27</v>
-      </c>
-      <c r="F61" t="s">
+      <c r="E61" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G61" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H61" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="I61" t="s">
+      <c r="I61" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="J61" t="s">
-        <v>15</v>
-      </c>
-      <c r="K61" t="s">
+      <c r="J61" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K61" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="L61" t="s">
+      <c r="L61" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M61" t="s">
+      <c r="M61" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N61" t="s">
-        <v>19</v>
-      </c>
-      <c r="O61" t="s">
-        <v>20</v>
-      </c>
-      <c r="P61" t="s">
+      <c r="N61" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O61" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P61" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B62">
+      <c r="B62" s="2">
         <v>61</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E62" t="s">
-        <v>27</v>
-      </c>
-      <c r="F62" t="s">
+      <c r="E62" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F62" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G62" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="H62" t="s">
+      <c r="H62" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="I62" t="s">
+      <c r="I62" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="J62" t="s">
-        <v>15</v>
-      </c>
-      <c r="K62" t="s">
+      <c r="J62" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K62" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="L62" t="s">
+      <c r="L62" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M62" t="s">
+      <c r="M62" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N62" t="s">
-        <v>19</v>
-      </c>
-      <c r="O62" t="s">
-        <v>20</v>
-      </c>
-      <c r="P62" t="s">
+      <c r="N62" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O62" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P62" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B63">
+      <c r="B63" s="2">
         <v>62</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E63" t="s">
-        <v>27</v>
-      </c>
-      <c r="F63" t="s">
+      <c r="E63" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F63" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G63" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="H63" t="s">
+      <c r="H63" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="I63" t="s">
+      <c r="I63" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="J63" t="s">
-        <v>15</v>
-      </c>
-      <c r="K63" t="s">
+      <c r="J63" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K63" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="L63" t="s">
+      <c r="L63" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M63" t="s">
+      <c r="M63" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N63" t="s">
-        <v>19</v>
-      </c>
-      <c r="O63" t="s">
-        <v>20</v>
-      </c>
-      <c r="P63" t="s">
+      <c r="N63" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O63" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P63" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B64">
+      <c r="B64" s="2">
         <v>63</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E64" t="s">
-        <v>27</v>
-      </c>
-      <c r="F64" t="s">
+      <c r="E64" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F64" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G64" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="H64" t="s">
+      <c r="H64" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="I64" t="s">
+      <c r="I64" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="J64" t="s">
-        <v>15</v>
-      </c>
-      <c r="K64" t="s">
+      <c r="J64" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K64" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L64" t="s">
+      <c r="L64" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="M64" t="s">
+      <c r="M64" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N64" t="s">
-        <v>19</v>
-      </c>
-      <c r="O64" t="s">
-        <v>20</v>
-      </c>
-      <c r="P64" t="s">
+      <c r="N64" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O64" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P64" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="65" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B65">
+      <c r="B65" s="2">
         <v>64</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E65" t="s">
-        <v>27</v>
-      </c>
-      <c r="F65" t="s">
+      <c r="E65" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F65" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="G65" t="s">
+      <c r="G65" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="H65" t="s">
+      <c r="H65" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="I65" t="s">
+      <c r="I65" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="J65" t="s">
-        <v>15</v>
-      </c>
-      <c r="K65" t="s">
+      <c r="J65" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K65" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="L65" t="s">
+      <c r="L65" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="M65" t="s">
+      <c r="M65" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N65" t="s">
-        <v>19</v>
-      </c>
-      <c r="O65" t="s">
-        <v>20</v>
-      </c>
-      <c r="P65" t="s">
+      <c r="N65" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O65" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P65" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="66" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B66">
+      <c r="B66" s="2">
         <v>65</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E66" t="s">
-        <v>27</v>
-      </c>
-      <c r="F66" t="s">
+      <c r="E66" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F66" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G66" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="H66" t="s">
+      <c r="H66" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="I66" t="s">
+      <c r="I66" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="J66" t="s">
-        <v>15</v>
-      </c>
-      <c r="K66" t="s">
+      <c r="J66" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K66" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="L66" t="s">
+      <c r="L66" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="M66" t="s">
+      <c r="M66" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N66" t="s">
-        <v>19</v>
-      </c>
-      <c r="O66" t="s">
-        <v>20</v>
-      </c>
-      <c r="P66" t="s">
+      <c r="N66" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O66" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P66" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="67" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B67">
+      <c r="B67" s="2">
         <v>66</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E67" t="s">
-        <v>27</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="E67" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="G67" t="s">
+      <c r="G67" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="H67" t="s">
+      <c r="H67" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="I67" t="s">
+      <c r="I67" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="J67" t="s">
-        <v>15</v>
-      </c>
-      <c r="K67" t="s">
+      <c r="J67" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K67" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="L67" t="s">
+      <c r="L67" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="M67" t="s">
+      <c r="M67" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N67" t="s">
-        <v>19</v>
-      </c>
-      <c r="O67" t="s">
-        <v>20</v>
-      </c>
-      <c r="P67" t="s">
+      <c r="N67" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O67" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P67" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="68" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B68">
+      <c r="B68" s="2">
         <v>67</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E68" t="s">
-        <v>27</v>
-      </c>
-      <c r="F68" t="s">
+      <c r="E68" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F68" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="G68" t="s">
+      <c r="G68" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="H68" t="s">
+      <c r="H68" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="I68" t="s">
+      <c r="I68" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="J68" t="s">
-        <v>15</v>
-      </c>
-      <c r="K68" t="s">
+      <c r="J68" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K68" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L68" t="s">
+      <c r="L68" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M68" t="s">
+      <c r="M68" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N68" t="s">
-        <v>19</v>
-      </c>
-      <c r="O68" t="s">
-        <v>20</v>
-      </c>
-      <c r="P68" t="s">
+      <c r="N68" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O68" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P68" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="69" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B69">
+      <c r="B69" s="2">
         <v>68</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E69" t="s">
-        <v>27</v>
-      </c>
-      <c r="F69" t="s">
+      <c r="E69" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="G69" t="s">
+      <c r="G69" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H69" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="I69" t="s">
+      <c r="I69" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="J69" t="s">
-        <v>15</v>
-      </c>
-      <c r="K69" t="s">
+      <c r="J69" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K69" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="L69" t="s">
+      <c r="L69" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M69" t="s">
+      <c r="M69" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N69" t="s">
-        <v>19</v>
-      </c>
-      <c r="O69" t="s">
-        <v>20</v>
-      </c>
-      <c r="P69" t="s">
+      <c r="N69" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O69" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P69" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="70" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B70">
+      <c r="B70" s="2">
         <v>69</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E70" t="s">
-        <v>27</v>
-      </c>
-      <c r="F70" t="s">
+      <c r="E70" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F70" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G70" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H70" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="I70" t="s">
+      <c r="I70" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="J70" t="s">
-        <v>15</v>
-      </c>
-      <c r="K70" t="s">
+      <c r="J70" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K70" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="L70" t="s">
+      <c r="L70" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M70" t="s">
+      <c r="M70" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N70" t="s">
-        <v>19</v>
-      </c>
-      <c r="O70" t="s">
-        <v>20</v>
-      </c>
-      <c r="P70" t="s">
+      <c r="N70" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O70" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P70" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="71" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B71">
+      <c r="B71" s="2">
         <v>70</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E71" t="s">
-        <v>27</v>
-      </c>
-      <c r="F71" t="s">
+      <c r="E71" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F71" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="G71" t="s">
+      <c r="G71" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="H71" t="s">
+      <c r="H71" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="I71" t="s">
+      <c r="I71" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="J71" t="s">
-        <v>15</v>
-      </c>
-      <c r="K71" t="s">
+      <c r="J71" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K71" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="L71" t="s">
+      <c r="L71" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M71" t="s">
+      <c r="M71" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N71" t="s">
-        <v>19</v>
-      </c>
-      <c r="O71" t="s">
-        <v>20</v>
-      </c>
-      <c r="P71" t="s">
+      <c r="N71" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O71" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P71" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="72" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B72">
+      <c r="B72" s="3">
         <v>71</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F72" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="G72" t="s">
+      <c r="G72" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="H72" t="s">
+      <c r="H72" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="I72" t="s">
+      <c r="I72" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="J72" t="s">
-        <v>15</v>
-      </c>
-      <c r="K72" t="s">
+      <c r="J72" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K72" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L72" t="s">
+      <c r="L72" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="M72" t="s">
+      <c r="M72" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N72" t="s">
-        <v>19</v>
-      </c>
-      <c r="O72" t="s">
-        <v>20</v>
-      </c>
-      <c r="P72" t="s">
+      <c r="N72" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O72" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P72" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="73" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B73">
+      <c r="B73" s="3">
         <v>72</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F73" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="G73" t="s">
+      <c r="G73" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="H73" t="s">
+      <c r="H73" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="I73" t="s">
+      <c r="I73" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="J73" t="s">
-        <v>15</v>
-      </c>
-      <c r="K73" t="s">
+      <c r="J73" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K73" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L73" t="s">
+      <c r="L73" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="M73" t="s">
+      <c r="M73" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N73" t="s">
-        <v>19</v>
-      </c>
-      <c r="O73" t="s">
-        <v>20</v>
-      </c>
-      <c r="P73" t="s">
+      <c r="N73" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O73" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P73" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="74" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B74">
+      <c r="B74" s="3">
         <v>73</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F74" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="G74" t="s">
+      <c r="G74" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="H74" t="s">
+      <c r="H74" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="I74" t="s">
+      <c r="I74" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="J74" t="s">
-        <v>15</v>
-      </c>
-      <c r="K74" t="s">
+      <c r="J74" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K74" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L74" t="s">
+      <c r="L74" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M74" t="s">
+      <c r="M74" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N74" t="s">
-        <v>19</v>
-      </c>
-      <c r="O74" t="s">
-        <v>20</v>
-      </c>
-      <c r="P74" t="s">
+      <c r="N74" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O74" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P74" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="75" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B75">
+      <c r="B75" s="3">
         <v>74</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F75" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="G75" t="s">
+      <c r="G75" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="H75" t="s">
+      <c r="H75" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="I75" t="s">
+      <c r="I75" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="J75" t="s">
-        <v>15</v>
-      </c>
-      <c r="K75" t="s">
+      <c r="J75" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K75" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L75" t="s">
+      <c r="L75" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="M75" t="s">
+      <c r="M75" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N75" t="s">
-        <v>19</v>
-      </c>
-      <c r="O75" t="s">
-        <v>20</v>
-      </c>
-      <c r="P75" t="s">
+      <c r="N75" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O75" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P75" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="76" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B76">
+      <c r="B76" s="3">
         <v>75</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="G76" t="s">
+      <c r="G76" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="H76" t="s">
+      <c r="H76" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="I76" t="s">
+      <c r="I76" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="J76" t="s">
-        <v>15</v>
-      </c>
-      <c r="K76" t="s">
+      <c r="J76" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K76" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L76" t="s">
+      <c r="L76" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="M76" t="s">
+      <c r="M76" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N76" t="s">
-        <v>19</v>
-      </c>
-      <c r="O76" t="s">
-        <v>20</v>
-      </c>
-      <c r="P76" t="s">
+      <c r="N76" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O76" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P76" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="77" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B77">
+      <c r="B77" s="4">
         <v>76</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F77" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="G77" t="s">
+      <c r="G77" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="H77" t="s">
+      <c r="H77" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="I77" t="s">
+      <c r="I77" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="J77" t="s">
-        <v>15</v>
-      </c>
-      <c r="K77" t="s">
+      <c r="J77" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K77" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L77" t="s">
+      <c r="L77" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M77" t="s">
+      <c r="M77" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N77" t="s">
-        <v>19</v>
-      </c>
-      <c r="O77" t="s">
-        <v>20</v>
-      </c>
-      <c r="P77" t="s">
+      <c r="N77" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O77" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P77" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="78" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B78">
+      <c r="B78" s="4">
         <v>77</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="G78" t="s">
+      <c r="G78" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="H78" t="s">
+      <c r="H78" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="I78" t="s">
+      <c r="I78" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="J78" t="s">
-        <v>15</v>
-      </c>
-      <c r="K78" t="s">
+      <c r="J78" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K78" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="L78" t="s">
+      <c r="L78" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M78" t="s">
+      <c r="M78" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N78" t="s">
-        <v>19</v>
-      </c>
-      <c r="O78" t="s">
-        <v>20</v>
-      </c>
-      <c r="P78" t="s">
+      <c r="N78" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O78" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P78" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="79" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B79">
+      <c r="B79" s="4">
         <v>78</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F79" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="G79" t="s">
+      <c r="G79" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="H79" t="s">
+      <c r="H79" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="I79" t="s">
+      <c r="I79" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="J79" t="s">
-        <v>15</v>
-      </c>
-      <c r="K79" t="s">
+      <c r="J79" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K79" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="L79" t="s">
+      <c r="L79" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M79" t="s">
+      <c r="M79" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N79" t="s">
-        <v>19</v>
-      </c>
-      <c r="O79" t="s">
-        <v>20</v>
-      </c>
-      <c r="P79" t="s">
+      <c r="N79" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O79" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P79" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="80" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B80">
+      <c r="B80" s="5">
         <v>79</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G80" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="H80" t="s">
+      <c r="H80" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="I80" t="s">
+      <c r="I80" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="J80" t="s">
-        <v>15</v>
-      </c>
-      <c r="K80" t="s">
+      <c r="J80" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K80" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L80" t="s">
+      <c r="L80" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="M80" t="s">
+      <c r="M80" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="N80" t="s">
-        <v>19</v>
-      </c>
-      <c r="O80" t="s">
-        <v>20</v>
-      </c>
-      <c r="P80" t="s">
+      <c r="N80" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O80" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P80" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="81" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B81">
+      <c r="B81" s="5">
         <v>80</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F81" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G81" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="H81" t="s">
+      <c r="H81" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="I81" t="s">
+      <c r="I81" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="J81" t="s">
-        <v>15</v>
-      </c>
-      <c r="K81" t="s">
+      <c r="J81" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K81" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="L81" t="s">
+      <c r="L81" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="M81" t="s">
+      <c r="M81" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="N81" t="s">
-        <v>19</v>
-      </c>
-      <c r="O81" t="s">
-        <v>20</v>
-      </c>
-      <c r="P81" t="s">
+      <c r="N81" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O81" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P81" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="82" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B82">
+      <c r="B82" s="5">
         <v>81</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D82" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F82" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G82" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="H82" t="s">
+      <c r="H82" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="I82" t="s">
+      <c r="I82" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="J82" t="s">
-        <v>15</v>
-      </c>
-      <c r="K82" t="s">
+      <c r="J82" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K82" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="L82" t="s">
+      <c r="L82" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="M82" t="s">
+      <c r="M82" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="N82" t="s">
-        <v>19</v>
-      </c>
-      <c r="O82" t="s">
-        <v>20</v>
-      </c>
-      <c r="P82" t="s">
+      <c r="N82" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O82" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P82" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="83" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B83">
+      <c r="B83" s="6">
         <v>82</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D83" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E83" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="G83" t="s">
+      <c r="G83" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="H83" t="s">
+      <c r="H83" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="I83" t="s">
+      <c r="I83" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="J83" t="s">
-        <v>15</v>
-      </c>
-      <c r="K83" t="s">
+      <c r="J83" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K83" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L83" t="s">
+      <c r="L83" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M83" t="s">
+      <c r="M83" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="N83" t="s">
-        <v>19</v>
-      </c>
-      <c r="O83" t="s">
-        <v>20</v>
-      </c>
-      <c r="P83" t="s">
+      <c r="N83" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O83" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="P83" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="84" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B84">
+      <c r="B84" s="6">
         <v>83</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E84" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F84" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G84" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="H84" t="s">
+      <c r="H84" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="I84" t="s">
+      <c r="I84" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="J84" t="s">
-        <v>15</v>
-      </c>
-      <c r="K84" t="s">
+      <c r="J84" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K84" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="L84" t="s">
+      <c r="L84" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M84" t="s">
+      <c r="M84" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="N84" t="s">
-        <v>19</v>
-      </c>
-      <c r="O84" t="s">
-        <v>20</v>
-      </c>
-      <c r="P84" t="s">
+      <c r="N84" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O84" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="P84" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="85" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B85">
+      <c r="B85" s="6">
         <v>84</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E85" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F85" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="G85" t="s">
+      <c r="G85" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="H85" t="s">
+      <c r="H85" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="I85" t="s">
+      <c r="I85" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="J85" t="s">
-        <v>15</v>
-      </c>
-      <c r="K85" t="s">
+      <c r="J85" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K85" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="L85" t="s">
+      <c r="L85" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M85" t="s">
+      <c r="M85" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="N85" t="s">
-        <v>19</v>
-      </c>
-      <c r="O85" t="s">
-        <v>20</v>
-      </c>
-      <c r="P85" t="s">
+      <c r="N85" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O85" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="P85" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="86" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B86">
+      <c r="B86" s="6">
         <v>85</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E86" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F86" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G86" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="H86" t="s">
+      <c r="H86" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="I86" t="s">
+      <c r="I86" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="J86" t="s">
-        <v>15</v>
-      </c>
-      <c r="K86" t="s">
+      <c r="J86" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K86" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="L86" t="s">
+      <c r="L86" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M86" t="s">
+      <c r="M86" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="N86" t="s">
-        <v>19</v>
-      </c>
-      <c r="O86" t="s">
-        <v>20</v>
-      </c>
-      <c r="P86" t="s">
+      <c r="N86" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O86" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="P86" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="87" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B87">
+      <c r="B87" s="7">
         <v>86</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E87" t="s">
-        <v>27</v>
-      </c>
-      <c r="F87" t="s">
+      <c r="E87" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F87" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G87" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="H87" t="s">
+      <c r="H87" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="I87" t="s">
+      <c r="I87" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="J87" t="s">
-        <v>15</v>
-      </c>
-      <c r="K87" t="s">
+      <c r="J87" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K87" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L87" t="s">
+      <c r="L87" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M87" t="s">
+      <c r="M87" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N87" t="s">
-        <v>19</v>
-      </c>
-      <c r="O87" t="s">
-        <v>20</v>
-      </c>
-      <c r="P87" t="s">
+      <c r="N87" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O87" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P87" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="88" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B88">
+      <c r="B88" s="7">
         <v>87</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="7" t="s">
         <v>382</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E88" t="s">
-        <v>27</v>
-      </c>
-      <c r="F88" t="s">
+      <c r="E88" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F88" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G88" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="H88" t="s">
+      <c r="H88" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="I88" t="s">
+      <c r="I88" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="J88" t="s">
-        <v>15</v>
-      </c>
-      <c r="K88" t="s">
+      <c r="J88" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K88" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="L88" t="s">
+      <c r="L88" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M88" t="s">
+      <c r="M88" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N88" t="s">
-        <v>19</v>
-      </c>
-      <c r="O88" t="s">
-        <v>20</v>
-      </c>
-      <c r="P88" t="s">
+      <c r="N88" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O88" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P88" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="89" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B89">
+      <c r="B89" s="7">
         <v>88</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E89" t="s">
-        <v>27</v>
-      </c>
-      <c r="F89" t="s">
+      <c r="E89" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F89" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="G89" t="s">
+      <c r="G89" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="H89" t="s">
+      <c r="H89" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="I89" t="s">
+      <c r="I89" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="J89" t="s">
-        <v>15</v>
-      </c>
-      <c r="K89" t="s">
+      <c r="J89" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K89" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="L89" t="s">
+      <c r="L89" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M89" t="s">
+      <c r="M89" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N89" t="s">
-        <v>19</v>
-      </c>
-      <c r="O89" t="s">
-        <v>20</v>
-      </c>
-      <c r="P89" t="s">
+      <c r="N89" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O89" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P89" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="90" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B90">
+      <c r="B90" s="7">
         <v>89</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E90" t="s">
-        <v>27</v>
-      </c>
-      <c r="F90" t="s">
+      <c r="E90" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F90" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G90" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="H90" t="s">
+      <c r="H90" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="I90" t="s">
+      <c r="I90" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="J90" t="s">
-        <v>15</v>
-      </c>
-      <c r="K90" t="s">
+      <c r="J90" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K90" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="L90" t="s">
+      <c r="L90" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M90" t="s">
+      <c r="M90" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N90" t="s">
-        <v>19</v>
-      </c>
-      <c r="O90" t="s">
-        <v>20</v>
-      </c>
-      <c r="P90" t="s">
+      <c r="N90" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O90" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P90" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="91" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B91">
+      <c r="B91" s="7">
         <v>90</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="7" t="s">
         <v>385</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E91" t="s">
-        <v>27</v>
-      </c>
-      <c r="F91" t="s">
+      <c r="E91" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F91" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="G91" t="s">
+      <c r="G91" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="H91" t="s">
+      <c r="H91" s="7" t="s">
         <v>364</v>
       </c>
-      <c r="I91" t="s">
+      <c r="I91" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="J91" t="s">
-        <v>15</v>
-      </c>
-      <c r="K91" t="s">
+      <c r="J91" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K91" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L91" t="s">
+      <c r="L91" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M91" t="s">
+      <c r="M91" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N91" t="s">
-        <v>19</v>
-      </c>
-      <c r="O91" t="s">
-        <v>20</v>
-      </c>
-      <c r="P91" t="s">
+      <c r="N91" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O91" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P91" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="92" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B92">
+      <c r="B92" s="7">
         <v>91</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E92" t="s">
-        <v>27</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="E92" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F92" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="G92" t="s">
+      <c r="G92" s="7" t="s">
         <v>365</v>
       </c>
-      <c r="H92" t="s">
+      <c r="H92" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="I92" t="s">
+      <c r="I92" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="J92" t="s">
-        <v>15</v>
-      </c>
-      <c r="K92" t="s">
+      <c r="J92" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K92" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L92" t="s">
+      <c r="L92" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M92" t="s">
+      <c r="M92" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N92" t="s">
-        <v>19</v>
-      </c>
-      <c r="O92" t="s">
-        <v>20</v>
-      </c>
-      <c r="P92" t="s">
+      <c r="N92" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O92" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P92" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="93" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B93">
+      <c r="B93" s="7">
         <v>92</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E93" t="s">
-        <v>27</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="E93" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F93" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G93" s="7" t="s">
         <v>370</v>
       </c>
-      <c r="H93" t="s">
+      <c r="H93" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="I93" t="s">
+      <c r="I93" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="J93" t="s">
-        <v>15</v>
-      </c>
-      <c r="K93" t="s">
+      <c r="J93" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K93" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L93" t="s">
+      <c r="L93" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M93" t="s">
+      <c r="M93" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N93" t="s">
-        <v>19</v>
-      </c>
-      <c r="O93" t="s">
-        <v>20</v>
-      </c>
-      <c r="P93" t="s">
+      <c r="N93" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O93" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P93" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="94" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B94">
+      <c r="B94" s="7">
         <v>93</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E94" t="s">
-        <v>27</v>
-      </c>
-      <c r="F94" t="s">
+      <c r="E94" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F94" s="7" t="s">
         <v>369</v>
       </c>
-      <c r="G94" t="s">
+      <c r="G94" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="H94" t="s">
+      <c r="H94" s="7" t="s">
         <v>373</v>
       </c>
-      <c r="I94" t="s">
+      <c r="I94" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="J94" t="s">
-        <v>15</v>
-      </c>
-      <c r="K94" t="s">
+      <c r="J94" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K94" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L94" t="s">
+      <c r="L94" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M94" t="s">
+      <c r="M94" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N94" t="s">
-        <v>19</v>
-      </c>
-      <c r="O94" t="s">
-        <v>20</v>
-      </c>
-      <c r="P94" t="s">
+      <c r="N94" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O94" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P94" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="95" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B95">
+      <c r="B95" s="7">
         <v>94</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E95" t="s">
-        <v>27</v>
-      </c>
-      <c r="F95" t="s">
+      <c r="E95" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F95" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G95" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="H95" t="s">
+      <c r="H95" s="7" t="s">
         <v>376</v>
       </c>
-      <c r="I95" t="s">
+      <c r="I95" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="J95" t="s">
-        <v>15</v>
-      </c>
-      <c r="K95" t="s">
+      <c r="J95" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K95" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L95" t="s">
+      <c r="L95" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M95" t="s">
+      <c r="M95" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N95" t="s">
-        <v>19</v>
-      </c>
-      <c r="O95" t="s">
-        <v>20</v>
-      </c>
-      <c r="P95" t="s">
+      <c r="N95" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O95" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P95" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="96" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B96">
+      <c r="B96" s="7">
         <v>95</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E96" t="s">
-        <v>27</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="E96" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F96" s="7" t="s">
         <v>374</v>
       </c>
-      <c r="G96" t="s">
+      <c r="G96" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="H96" t="s">
+      <c r="H96" s="7" t="s">
         <v>379</v>
       </c>
-      <c r="I96" t="s">
+      <c r="I96" s="7" t="s">
         <v>380</v>
       </c>
-      <c r="J96" t="s">
-        <v>15</v>
-      </c>
-      <c r="K96" t="s">
+      <c r="J96" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K96" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L96" t="s">
+      <c r="L96" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M96" t="s">
+      <c r="M96" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N96" t="s">
-        <v>19</v>
-      </c>
-      <c r="O96" t="s">
-        <v>20</v>
-      </c>
-      <c r="P96" t="s">
+      <c r="N96" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O96" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P96" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B97">
+      <c r="B97" s="7">
         <v>96</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E97" t="s">
-        <v>27</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="E97" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F97" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="G97" t="s">
+      <c r="G97" s="7" t="s">
         <v>392</v>
       </c>
-      <c r="H97" t="s">
+      <c r="H97" s="7" t="s">
         <v>393</v>
       </c>
-      <c r="I97" t="s">
+      <c r="I97" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="J97" t="s">
-        <v>15</v>
-      </c>
-      <c r="K97" t="s">
+      <c r="J97" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K97" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L97" t="s">
+      <c r="L97" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M97" t="s">
+      <c r="M97" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N97" t="s">
-        <v>19</v>
-      </c>
-      <c r="O97" t="s">
-        <v>20</v>
-      </c>
-      <c r="P97" t="s">
+      <c r="N97" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O97" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P97" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B98">
+      <c r="B98" s="7">
         <v>97</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E98" t="s">
-        <v>27</v>
-      </c>
-      <c r="F98" t="s">
+      <c r="E98" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F98" s="7" t="s">
         <v>395</v>
       </c>
-      <c r="G98" t="s">
+      <c r="G98" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="H98" t="s">
+      <c r="H98" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="I98" t="s">
+      <c r="I98" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="J98" t="s">
-        <v>15</v>
-      </c>
-      <c r="K98" t="s">
+      <c r="J98" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K98" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L98" t="s">
+      <c r="L98" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M98" t="s">
+      <c r="M98" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N98" t="s">
-        <v>19</v>
-      </c>
-      <c r="O98" t="s">
-        <v>20</v>
-      </c>
-      <c r="P98" t="s">
+      <c r="N98" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O98" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P98" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B99">
+      <c r="B99" s="7">
         <v>98</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E99" t="s">
-        <v>27</v>
-      </c>
-      <c r="F99" t="s">
+      <c r="E99" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F99" s="7" t="s">
         <v>400</v>
       </c>
-      <c r="G99" t="s">
+      <c r="G99" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="H99" t="s">
+      <c r="H99" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="I99" t="s">
+      <c r="I99" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="J99" t="s">
-        <v>15</v>
-      </c>
-      <c r="K99" t="s">
+      <c r="J99" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K99" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L99" t="s">
+      <c r="L99" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M99" t="s">
+      <c r="M99" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N99" t="s">
-        <v>19</v>
-      </c>
-      <c r="O99" t="s">
-        <v>20</v>
-      </c>
-      <c r="P99" t="s">
+      <c r="N99" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O99" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P99" s="7" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>